<commit_message>
Updated the pandas examples
</commit_message>
<xml_diff>
--- a/Pandas/pandas/ex2.xlsx
+++ b/Pandas/pandas/ex2.xlsx
@@ -450,10 +450,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>-0.6770571948988893</v>
+        <v>-0.6436936677321438</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.7625113330861892</v>
+        <v>0.6048615524379573</v>
       </c>
     </row>
     <row r="3">
@@ -461,10 +461,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.8261860367873372</v>
+        <v>0.8481987922759403</v>
       </c>
       <c r="C3" t="n">
-        <v>0.5270267454904476</v>
+        <v>-0.06183975955357971</v>
       </c>
     </row>
     <row r="4">
@@ -472,10 +472,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>-1.224187344211913</v>
+        <v>0.1362243115762983</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.5829991199055904</v>
+        <v>0.6668242860948045</v>
       </c>
     </row>
     <row r="5">
@@ -483,10 +483,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.1426796409713911</v>
+        <v>-2.866014234017723</v>
       </c>
       <c r="C5" t="n">
-        <v>0.5347626007058357</v>
+        <v>1.427542058963176</v>
       </c>
     </row>
     <row r="6">
@@ -494,10 +494,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>0.4835678367074906</v>
+        <v>-0.4341914718821441</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.2055425614900198</v>
+        <v>-1.875270068897947</v>
       </c>
     </row>
     <row r="7">
@@ -505,10 +505,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>0.04134968172942036</v>
+        <v>-1.448678003288501</v>
       </c>
       <c r="C7" t="n">
-        <v>-1.141230291740927</v>
+        <v>-0.7410904468199772</v>
       </c>
     </row>
     <row r="8">
@@ -516,10 +516,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>2.085288540438845</v>
+        <v>-2.670841336409842</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.9346107924197017</v>
+        <v>0.3023040868638705</v>
       </c>
     </row>
     <row r="9">
@@ -527,10 +527,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>-0.9312120217679818</v>
+        <v>0.253343792392148</v>
       </c>
       <c r="C9" t="n">
-        <v>0.00847937277796949</v>
+        <v>0.3395936605247907</v>
       </c>
     </row>
     <row r="10">
@@ -538,10 +538,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>2.631864726108758</v>
+        <v>1.124378825728025</v>
       </c>
       <c r="C10" t="n">
-        <v>1.280038823108819</v>
+        <v>0.5815546117344512</v>
       </c>
     </row>
     <row r="11">
@@ -549,10 +549,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>0.5252325398444225</v>
+        <v>-0.3328171023833046</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.1606475022754813</v>
+        <v>-0.734141001411168</v>
       </c>
     </row>
     <row r="12">
@@ -560,10 +560,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>0.2448155428398311</v>
+        <v>0.9715251082647074</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.7384312816646994</v>
+        <v>-0.5451462484222711</v>
       </c>
     </row>
     <row r="13">
@@ -571,10 +571,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>0.4386656449069076</v>
+        <v>-0.3151471034450695</v>
       </c>
       <c r="C13" t="n">
-        <v>-0.1531943401682386</v>
+        <v>0.9682226724522393</v>
       </c>
     </row>
     <row r="14">
@@ -582,10 +582,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>-0.05454365238797751</v>
+        <v>-0.4595775492837924</v>
       </c>
       <c r="C14" t="n">
-        <v>0.6174815707299837</v>
+        <v>0.8289935256924429</v>
       </c>
     </row>
     <row r="15">
@@ -593,10 +593,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>0.755347516529725</v>
+        <v>0.6593929085579789</v>
       </c>
       <c r="C15" t="n">
-        <v>-0.3057273756605429</v>
+        <v>-2.243730152265649</v>
       </c>
     </row>
     <row r="16">
@@ -604,10 +604,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>-0.067433971641289</v>
+        <v>-0.07791176058193165</v>
       </c>
       <c r="C16" t="n">
-        <v>1.688032554695911</v>
+        <v>-0.6495241628031473</v>
       </c>
     </row>
     <row r="17">
@@ -615,10 +615,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>0.5242377178463442</v>
+        <v>0.1686142624598296</v>
       </c>
       <c r="C17" t="n">
-        <v>0.2296559644198027</v>
+        <v>0.191724201537998</v>
       </c>
     </row>
     <row r="18">
@@ -626,10 +626,10 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>-0.9247551010009074</v>
+        <v>2.382645102519338</v>
       </c>
       <c r="C18" t="n">
-        <v>-0.7463077600412145</v>
+        <v>-0.4582057661330416</v>
       </c>
     </row>
     <row r="19">
@@ -637,10 +637,10 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>-1.233579523378663</v>
+        <v>0.550240542470282</v>
       </c>
       <c r="C19" t="n">
-        <v>-0.9000805157108368</v>
+        <v>1.436781058176872</v>
       </c>
     </row>
     <row r="20">
@@ -648,10 +648,10 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>-0.3872493600659856</v>
+        <v>-1.32313431129281</v>
       </c>
       <c r="C20" t="n">
-        <v>0.2454502924988893</v>
+        <v>-2.230893663151085</v>
       </c>
     </row>
     <row r="21">
@@ -659,10 +659,10 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>-0.01581004899677589</v>
+        <v>0.1201625389229685</v>
       </c>
       <c r="C21" t="n">
-        <v>-1.481529501392181</v>
+        <v>0.6169262894177493</v>
       </c>
     </row>
     <row r="22">
@@ -670,10 +670,10 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>-0.398938077326145</v>
+        <v>-1.238371232078775</v>
       </c>
       <c r="C22" t="n">
-        <v>0.4156005548091177</v>
+        <v>-0.3955137710785661</v>
       </c>
     </row>
     <row r="23">
@@ -681,10 +681,10 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>-0.1097720097512328</v>
+        <v>-1.794652629800652</v>
       </c>
       <c r="C23" t="n">
-        <v>-1.304516622904589</v>
+        <v>2.468249722939703</v>
       </c>
     </row>
     <row r="24">
@@ -692,10 +692,10 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>1.010055816561504</v>
+        <v>-0.0836666869437588</v>
       </c>
       <c r="C24" t="n">
-        <v>-0.6887023992830864</v>
+        <v>-0.9638709116197721</v>
       </c>
     </row>
     <row r="25">
@@ -703,10 +703,10 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>-0.3984616399033167</v>
+        <v>-1.479878989264926</v>
       </c>
       <c r="C25" t="n">
-        <v>1.141748978888797</v>
+        <v>0.3508202005104995</v>
       </c>
     </row>
     <row r="26">
@@ -714,10 +714,10 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>-0.8148289154096663</v>
+        <v>1.482014008149077</v>
       </c>
       <c r="C26" t="n">
-        <v>0.4656048883953414</v>
+        <v>0.7554382049861887</v>
       </c>
     </row>
     <row r="27">
@@ -725,10 +725,10 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>-1.178600902591018</v>
+        <v>-0.4152403562579223</v>
       </c>
       <c r="C27" t="n">
-        <v>0.5896577846417664</v>
+        <v>1.148642674641205</v>
       </c>
     </row>
     <row r="28">
@@ -736,10 +736,10 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>-0.4199855930195884</v>
+        <v>1.123590593476252</v>
       </c>
       <c r="C28" t="n">
-        <v>-0.5903476779239573</v>
+        <v>-1.060910880374953</v>
       </c>
     </row>
     <row r="29">
@@ -747,10 +747,10 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>0.4193537740733876</v>
+        <v>0.1594692143239325</v>
       </c>
       <c r="C29" t="n">
-        <v>-0.7237317886263034</v>
+        <v>1.221488544430398</v>
       </c>
     </row>
     <row r="30">
@@ -758,10 +758,10 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>-2.845782234943655</v>
+        <v>-0.2933732025751061</v>
       </c>
       <c r="C30" t="n">
-        <v>-0.5658216842619751</v>
+        <v>-0.214152447243255</v>
       </c>
     </row>
     <row r="31">
@@ -769,10 +769,10 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>-1.026871244356326</v>
+        <v>-0.8855557045211763</v>
       </c>
       <c r="C31" t="n">
-        <v>0.8564781214860402</v>
+        <v>1.020915229079611</v>
       </c>
     </row>
     <row r="32">
@@ -780,10 +780,10 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>-1.440081196678597</v>
+        <v>0.0620496432929693</v>
       </c>
       <c r="C32" t="n">
-        <v>0.01215916593993853</v>
+        <v>0.3544165865739892</v>
       </c>
     </row>
     <row r="33">
@@ -791,10 +791,10 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>0.8877056790525735</v>
+        <v>-1.3702988547915</v>
       </c>
       <c r="C33" t="n">
-        <v>0.1702662717595553</v>
+        <v>-0.6461119001904715</v>
       </c>
     </row>
     <row r="34">
@@ -802,10 +802,10 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>-1.099252205975928</v>
+        <v>-1.754582786087739</v>
       </c>
       <c r="C34" t="n">
-        <v>1.221254146617138</v>
+        <v>-0.3991244150749291</v>
       </c>
     </row>
     <row r="35">
@@ -813,10 +813,10 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>-0.317181416788784</v>
+        <v>0.5664072676744579</v>
       </c>
       <c r="C35" t="n">
-        <v>-0.1342343728657678</v>
+        <v>-1.480385013511401</v>
       </c>
     </row>
     <row r="36">
@@ -824,10 +824,10 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>-0.3799922246334332</v>
+        <v>1.445166997699438</v>
       </c>
       <c r="C36" t="n">
-        <v>-1.262631947926941</v>
+        <v>-1.639949060347753</v>
       </c>
     </row>
     <row r="37">
@@ -835,10 +835,10 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>-0.4302452617898552</v>
+        <v>0.4459971448962949</v>
       </c>
       <c r="C37" t="n">
-        <v>0.4722092111756401</v>
+        <v>-0.5379657233611839</v>
       </c>
     </row>
     <row r="38">
@@ -846,10 +846,10 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>-2.062010977287495</v>
+        <v>-1.565073502983542</v>
       </c>
       <c r="C38" t="n">
-        <v>1.131221604628871</v>
+        <v>-0.6950834099672214</v>
       </c>
     </row>
     <row r="39">
@@ -857,10 +857,10 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>-0.6184963933885366</v>
+        <v>0.2463880731422886</v>
       </c>
       <c r="C39" t="n">
-        <v>-0.7948296883612915</v>
+        <v>-0.2477069577402639</v>
       </c>
     </row>
     <row r="40">
@@ -868,10 +868,10 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>-0.07184241765671651</v>
+        <v>-0.3507242913887475</v>
       </c>
       <c r="C40" t="n">
-        <v>0.08589987797833235</v>
+        <v>-1.44051868664003</v>
       </c>
     </row>
     <row r="41">
@@ -879,10 +879,10 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>2.353204326513785</v>
+        <v>-0.6514460131826214</v>
       </c>
       <c r="C41" t="n">
-        <v>1.291232720427156</v>
+        <v>-0.6292782376388897</v>
       </c>
     </row>
     <row r="42">
@@ -890,10 +890,10 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>-0.5231111839791905</v>
+        <v>-0.5464757699054879</v>
       </c>
       <c r="C42" t="n">
-        <v>-0.4159916806495094</v>
+        <v>-0.1714765588734759</v>
       </c>
     </row>
     <row r="43">
@@ -901,10 +901,10 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>-0.56478454005564</v>
+        <v>0.3231629392285399</v>
       </c>
       <c r="C43" t="n">
-        <v>1.135379881120791</v>
+        <v>0.6534159802800087</v>
       </c>
     </row>
     <row r="44">
@@ -912,10 +912,10 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>0.1554548571668218</v>
+        <v>-0.2915282051470537</v>
       </c>
       <c r="C44" t="n">
-        <v>1.37735989787243</v>
+        <v>0.6967750831528265</v>
       </c>
     </row>
     <row r="45">
@@ -923,10 +923,10 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>-0.6603378194263264</v>
+        <v>0.6151820722118405</v>
       </c>
       <c r="C45" t="n">
-        <v>-0.7514773194839574</v>
+        <v>1.091175472278164</v>
       </c>
     </row>
     <row r="46">
@@ -934,10 +934,10 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>-0.1123768938156212</v>
+        <v>2.588000478193001</v>
       </c>
       <c r="C46" t="n">
-        <v>1.365257456169539</v>
+        <v>-0.04589524596991784</v>
       </c>
     </row>
     <row r="47">
@@ -945,10 +945,10 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>-0.3139306241637557</v>
+        <v>1.370749451107059</v>
       </c>
       <c r="C47" t="n">
-        <v>1.199156511278655</v>
+        <v>-1.178660215603311</v>
       </c>
     </row>
     <row r="48">
@@ -956,10 +956,10 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>-0.5162022816621806</v>
+        <v>0.9393252668458343</v>
       </c>
       <c r="C48" t="n">
-        <v>0.3445871207323281</v>
+        <v>-1.355580438879415</v>
       </c>
     </row>
     <row r="49">
@@ -967,10 +967,10 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>0.3203838183303547</v>
+        <v>0.3006316064031579</v>
       </c>
       <c r="C49" t="n">
-        <v>-0.1038169562891925</v>
+        <v>0.771349844936364</v>
       </c>
     </row>
     <row r="50">
@@ -978,10 +978,10 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>0.9887146778817342</v>
+        <v>0.05815274417296564</v>
       </c>
       <c r="C50" t="n">
-        <v>0.1109262549327307</v>
+        <v>2.246041315098033</v>
       </c>
     </row>
     <row r="51">
@@ -989,10 +989,10 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>0.2003664595380358</v>
+        <v>0.5267149621358643</v>
       </c>
       <c r="C51" t="n">
-        <v>-2.022748086461025</v>
+        <v>0.8233417008525109</v>
       </c>
     </row>
     <row r="52">
@@ -1000,10 +1000,10 @@
         <v>50</v>
       </c>
       <c r="B52" t="n">
-        <v>-0.4968682403797104</v>
+        <v>-0.7123731816434228</v>
       </c>
       <c r="C52" t="n">
-        <v>-0.04106722575363769</v>
+        <v>0.276469818975218</v>
       </c>
     </row>
     <row r="53">
@@ -1011,10 +1011,10 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>-0.6258625049890603</v>
+        <v>0.8581973449076185</v>
       </c>
       <c r="C53" t="n">
-        <v>0.07863594215053653</v>
+        <v>0.2413355351084589</v>
       </c>
     </row>
     <row r="54">
@@ -1022,10 +1022,10 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>-1.413001962705386</v>
+        <v>-1.145956704531524</v>
       </c>
       <c r="C54" t="n">
-        <v>1.769675812981382</v>
+        <v>-1.226158624623136</v>
       </c>
     </row>
     <row r="55">
@@ -1033,10 +1033,10 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>1.383048474753168</v>
+        <v>0.5361686707597</v>
       </c>
       <c r="C55" t="n">
-        <v>1.106825994935127</v>
+        <v>-0.2499597238895034</v>
       </c>
     </row>
     <row r="56">
@@ -1044,10 +1044,10 @@
         <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>-1.064875913492042</v>
+        <v>0.7660601344380447</v>
       </c>
       <c r="C56" t="n">
-        <v>0.08558462056297472</v>
+        <v>0.6634042422292832</v>
       </c>
     </row>
     <row r="57">
@@ -1055,10 +1055,10 @@
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>-0.3928313574184342</v>
+        <v>-0.9432762958309731</v>
       </c>
       <c r="C57" t="n">
-        <v>0.7768832680676769</v>
+        <v>0.2823738417461684</v>
       </c>
     </row>
     <row r="58">
@@ -1066,10 +1066,10 @@
         <v>56</v>
       </c>
       <c r="B58" t="n">
-        <v>-1.195871976797731</v>
+        <v>-0.837221143630809</v>
       </c>
       <c r="C58" t="n">
-        <v>-0.5694546808128571</v>
+        <v>-0.8561477056658795</v>
       </c>
     </row>
     <row r="59">
@@ -1077,10 +1077,10 @@
         <v>57</v>
       </c>
       <c r="B59" t="n">
-        <v>-1.987609712535389</v>
+        <v>-0.8351698402828253</v>
       </c>
       <c r="C59" t="n">
-        <v>-0.3676692867577258</v>
+        <v>0.8263068678054736</v>
       </c>
     </row>
     <row r="60">
@@ -1088,10 +1088,10 @@
         <v>58</v>
       </c>
       <c r="B60" t="n">
-        <v>0.9671235492252669</v>
+        <v>0.1419408932370512</v>
       </c>
       <c r="C60" t="n">
-        <v>-0.1837116137256158</v>
+        <v>-1.495064388596024</v>
       </c>
     </row>
     <row r="61">
@@ -1099,10 +1099,10 @@
         <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>-0.1404666670833804</v>
+        <v>0.3022392408561329</v>
       </c>
       <c r="C61" t="n">
-        <v>-0.577528509578495</v>
+        <v>-0.3825669144857662</v>
       </c>
     </row>
     <row r="62">
@@ -1110,10 +1110,10 @@
         <v>60</v>
       </c>
       <c r="B62" t="n">
-        <v>0.5097240484238101</v>
+        <v>-0.4127490461341597</v>
       </c>
       <c r="C62" t="n">
-        <v>0.170497123500247</v>
+        <v>-0.6458329774761561</v>
       </c>
     </row>
     <row r="63">
@@ -1121,10 +1121,10 @@
         <v>61</v>
       </c>
       <c r="B63" t="n">
-        <v>2.457300131350754</v>
+        <v>-2.085492571584192</v>
       </c>
       <c r="C63" t="n">
-        <v>1.322546518685465</v>
+        <v>0.3716365098571095</v>
       </c>
     </row>
     <row r="64">
@@ -1132,10 +1132,10 @@
         <v>62</v>
       </c>
       <c r="B64" t="n">
-        <v>1.671449581450998</v>
+        <v>0.1315193023423922</v>
       </c>
       <c r="C64" t="n">
-        <v>0.3048501914197734</v>
+        <v>1.222406872154715</v>
       </c>
     </row>
     <row r="65">
@@ -1143,10 +1143,10 @@
         <v>63</v>
       </c>
       <c r="B65" t="n">
-        <v>0.8526309224411892</v>
+        <v>-0.2386606521516989</v>
       </c>
       <c r="C65" t="n">
-        <v>0.4707143917532779</v>
+        <v>0.5866952124266063</v>
       </c>
     </row>
     <row r="66">
@@ -1154,10 +1154,10 @@
         <v>64</v>
       </c>
       <c r="B66" t="n">
-        <v>-0.01195848325745125</v>
+        <v>0.2617963838242409</v>
       </c>
       <c r="C66" t="n">
-        <v>1.308643922864158</v>
+        <v>0.06977936609247397</v>
       </c>
     </row>
     <row r="67">
@@ -1165,10 +1165,10 @@
         <v>65</v>
       </c>
       <c r="B67" t="n">
-        <v>0.3432257401980983</v>
+        <v>-0.6241851056429294</v>
       </c>
       <c r="C67" t="n">
-        <v>-0.001390982037932893</v>
+        <v>-1.037653362277436</v>
       </c>
     </row>
     <row r="68">
@@ -1176,10 +1176,10 @@
         <v>66</v>
       </c>
       <c r="B68" t="n">
-        <v>0.722836376421248</v>
+        <v>-0.4539420747994777</v>
       </c>
       <c r="C68" t="n">
-        <v>0.08212184658176658</v>
+        <v>1.30576054228318</v>
       </c>
     </row>
     <row r="69">
@@ -1187,10 +1187,10 @@
         <v>67</v>
       </c>
       <c r="B69" t="n">
-        <v>1.331389498833376</v>
+        <v>-0.404701238277281</v>
       </c>
       <c r="C69" t="n">
-        <v>-1.77834518532638</v>
+        <v>1.075223412767373</v>
       </c>
     </row>
     <row r="70">
@@ -1198,10 +1198,10 @@
         <v>68</v>
       </c>
       <c r="B70" t="n">
-        <v>0.4244914063837149</v>
+        <v>1.235252177085605</v>
       </c>
       <c r="C70" t="n">
-        <v>-0.4809561319830208</v>
+        <v>-0.8031512192257261</v>
       </c>
     </row>
     <row r="71">
@@ -1209,10 +1209,10 @@
         <v>69</v>
       </c>
       <c r="B71" t="n">
-        <v>-0.5313954144142407</v>
+        <v>0.09702201463857606</v>
       </c>
       <c r="C71" t="n">
-        <v>-0.754528271531717</v>
+        <v>1.453845934993659</v>
       </c>
     </row>
     <row r="72">
@@ -1220,10 +1220,10 @@
         <v>70</v>
       </c>
       <c r="B72" t="n">
-        <v>-0.518939235136252</v>
+        <v>-0.09487154581914876</v>
       </c>
       <c r="C72" t="n">
-        <v>-1.144789131793179</v>
+        <v>1.814408098157268</v>
       </c>
     </row>
     <row r="73">
@@ -1231,10 +1231,10 @@
         <v>71</v>
       </c>
       <c r="B73" t="n">
-        <v>0.6761065839823478</v>
+        <v>0.2271801367917244</v>
       </c>
       <c r="C73" t="n">
-        <v>0.0294433307660455</v>
+        <v>-1.115393088223188</v>
       </c>
     </row>
     <row r="74">
@@ -1242,10 +1242,10 @@
         <v>72</v>
       </c>
       <c r="B74" t="n">
-        <v>1.159272542169936</v>
+        <v>0.9328267110342523</v>
       </c>
       <c r="C74" t="n">
-        <v>2.185684691190448</v>
+        <v>2.168521318056309</v>
       </c>
     </row>
     <row r="75">
@@ -1253,10 +1253,10 @@
         <v>73</v>
       </c>
       <c r="B75" t="n">
-        <v>-0.03593991853454029</v>
+        <v>-0.09315705105604782</v>
       </c>
       <c r="C75" t="n">
-        <v>0.8075361142029329</v>
+        <v>-0.345436021703852</v>
       </c>
     </row>
     <row r="76">
@@ -1264,10 +1264,10 @@
         <v>74</v>
       </c>
       <c r="B76" t="n">
-        <v>1.456970961966452</v>
+        <v>1.878318642470408</v>
       </c>
       <c r="C76" t="n">
-        <v>0.2711483225120178</v>
+        <v>1.116318477641528</v>
       </c>
     </row>
     <row r="77">
@@ -1275,10 +1275,10 @@
         <v>75</v>
       </c>
       <c r="B77" t="n">
-        <v>-0.7884790249174076</v>
+        <v>0.1932647763661189</v>
       </c>
       <c r="C77" t="n">
-        <v>-0.6745608497145797</v>
+        <v>-0.5724231192636764</v>
       </c>
     </row>
     <row r="78">
@@ -1286,10 +1286,10 @@
         <v>76</v>
       </c>
       <c r="B78" t="n">
-        <v>-0.3009445944298026</v>
+        <v>0.1912617951639147</v>
       </c>
       <c r="C78" t="n">
-        <v>1.651360805700889</v>
+        <v>-0.6834481631749896</v>
       </c>
     </row>
     <row r="79">
@@ -1297,10 +1297,10 @@
         <v>77</v>
       </c>
       <c r="B79" t="n">
-        <v>0.3515883806500118</v>
+        <v>-0.2693225846762528</v>
       </c>
       <c r="C79" t="n">
-        <v>-0.188522320173198</v>
+        <v>0.4378468894079781</v>
       </c>
     </row>
     <row r="80">
@@ -1308,10 +1308,10 @@
         <v>78</v>
       </c>
       <c r="B80" t="n">
-        <v>1.507556010714401</v>
+        <v>0.5623434878191472</v>
       </c>
       <c r="C80" t="n">
-        <v>0.2187626915236574</v>
+        <v>0.3404363215159713</v>
       </c>
     </row>
     <row r="81">
@@ -1319,10 +1319,10 @@
         <v>79</v>
       </c>
       <c r="B81" t="n">
-        <v>-0.3866853014390395</v>
+        <v>-0.8391119319658223</v>
       </c>
       <c r="C81" t="n">
-        <v>-1.678238027285777</v>
+        <v>-1.456319730170735</v>
       </c>
     </row>
     <row r="82">
@@ -1330,10 +1330,10 @@
         <v>80</v>
       </c>
       <c r="B82" t="n">
-        <v>0.7584735319493205</v>
+        <v>-1.948869760072637</v>
       </c>
       <c r="C82" t="n">
-        <v>0.6189143717758347</v>
+        <v>-0.1042592799032529</v>
       </c>
     </row>
     <row r="83">
@@ -1341,10 +1341,10 @@
         <v>81</v>
       </c>
       <c r="B83" t="n">
-        <v>-1.495602791128681</v>
+        <v>-1.44804662971959</v>
       </c>
       <c r="C83" t="n">
-        <v>-0.1066516208332936</v>
+        <v>-0.02036165746055315</v>
       </c>
     </row>
     <row r="84">
@@ -1352,10 +1352,10 @@
         <v>82</v>
       </c>
       <c r="B84" t="n">
-        <v>-0.350014568950799</v>
+        <v>0.06947472423285476</v>
       </c>
       <c r="C84" t="n">
-        <v>-0.19837845021407</v>
+        <v>0.3447790295087322</v>
       </c>
     </row>
     <row r="85">
@@ -1363,10 +1363,10 @@
         <v>83</v>
       </c>
       <c r="B85" t="n">
-        <v>-0.9838456455217944</v>
+        <v>0.03229711418411784</v>
       </c>
       <c r="C85" t="n">
-        <v>0.2273739704461027</v>
+        <v>-1.180213158933638</v>
       </c>
     </row>
     <row r="86">
@@ -1374,10 +1374,10 @@
         <v>84</v>
       </c>
       <c r="B86" t="n">
-        <v>0.3527980049016811</v>
+        <v>-0.03350886978972536</v>
       </c>
       <c r="C86" t="n">
-        <v>0.6678307726666336</v>
+        <v>0.03624222666411998</v>
       </c>
     </row>
     <row r="87">
@@ -1385,10 +1385,10 @@
         <v>85</v>
       </c>
       <c r="B87" t="n">
-        <v>0.1329487694619317</v>
+        <v>0.7344473818902533</v>
       </c>
       <c r="C87" t="n">
-        <v>-0.430003486929001</v>
+        <v>-0.510248074893689</v>
       </c>
     </row>
     <row r="88">
@@ -1396,10 +1396,10 @@
         <v>86</v>
       </c>
       <c r="B88" t="n">
-        <v>1.360555192824605</v>
+        <v>-1.092627473367835</v>
       </c>
       <c r="C88" t="n">
-        <v>-0.7095637295835023</v>
+        <v>-0.7863097810137865</v>
       </c>
     </row>
     <row r="89">
@@ -1407,10 +1407,10 @@
         <v>87</v>
       </c>
       <c r="B89" t="n">
-        <v>2.302571799227787</v>
+        <v>0.5658131615087325</v>
       </c>
       <c r="C89" t="n">
-        <v>-0.0008437569490138963</v>
+        <v>1.195582748791698</v>
       </c>
     </row>
     <row r="90">
@@ -1418,10 +1418,10 @@
         <v>88</v>
       </c>
       <c r="B90" t="n">
-        <v>0.0241481332333052</v>
+        <v>0.755411988513544</v>
       </c>
       <c r="C90" t="n">
-        <v>-1.151094422844163</v>
+        <v>0.1232495374633156</v>
       </c>
     </row>
     <row r="91">
@@ -1429,10 +1429,10 @@
         <v>89</v>
       </c>
       <c r="B91" t="n">
-        <v>1.637387265272397</v>
+        <v>-0.678145361754754</v>
       </c>
       <c r="C91" t="n">
-        <v>1.30438169390306</v>
+        <v>-1.102240414597044</v>
       </c>
     </row>
     <row r="92">
@@ -1440,10 +1440,10 @@
         <v>90</v>
       </c>
       <c r="B92" t="n">
-        <v>-2.446322874131691</v>
+        <v>-1.916282923517614</v>
       </c>
       <c r="C92" t="n">
-        <v>-0.5452617041821125</v>
+        <v>0.7102227163283419</v>
       </c>
     </row>
     <row r="93">
@@ -1451,10 +1451,10 @@
         <v>91</v>
       </c>
       <c r="B93" t="n">
-        <v>1.355550354820176</v>
+        <v>-0.8248177828102289</v>
       </c>
       <c r="C93" t="n">
-        <v>-0.6719875667830757</v>
+        <v>0.3554956757573015</v>
       </c>
     </row>
     <row r="94">
@@ -1462,10 +1462,10 @@
         <v>92</v>
       </c>
       <c r="B94" t="n">
-        <v>1.715941490700171</v>
+        <v>1.228226554465794</v>
       </c>
       <c r="C94" t="n">
-        <v>1.417919063284305</v>
+        <v>0.03827843410827805</v>
       </c>
     </row>
     <row r="95">
@@ -1473,10 +1473,10 @@
         <v>93</v>
       </c>
       <c r="B95" t="n">
-        <v>-0.4404333753664166</v>
+        <v>-0.5431044208630181</v>
       </c>
       <c r="C95" t="n">
-        <v>0.1422223999842894</v>
+        <v>-1.12796578461849</v>
       </c>
     </row>
     <row r="96">
@@ -1484,10 +1484,10 @@
         <v>94</v>
       </c>
       <c r="B96" t="n">
-        <v>-0.5330569253506127</v>
+        <v>0.3684630369346275</v>
       </c>
       <c r="C96" t="n">
-        <v>-0.4371440165112341</v>
+        <v>1.277668742749809</v>
       </c>
     </row>
     <row r="97">
@@ -1495,10 +1495,10 @@
         <v>95</v>
       </c>
       <c r="B97" t="n">
-        <v>1.576342541141162</v>
+        <v>1.287616710102915</v>
       </c>
       <c r="C97" t="n">
-        <v>0.5759541894386302</v>
+        <v>-0.5011707599454829</v>
       </c>
     </row>
     <row r="98">
@@ -1506,10 +1506,10 @@
         <v>96</v>
       </c>
       <c r="B98" t="n">
-        <v>0.4283580864850136</v>
+        <v>-0.07176661507610869</v>
       </c>
       <c r="C98" t="n">
-        <v>-0.680549380620951</v>
+        <v>1.301262065439911</v>
       </c>
     </row>
     <row r="99">
@@ -1517,10 +1517,10 @@
         <v>97</v>
       </c>
       <c r="B99" t="n">
-        <v>1.230585575986001</v>
+        <v>0.7745833125790254</v>
       </c>
       <c r="C99" t="n">
-        <v>0.1798213111625755</v>
+        <v>-0.7349295588644752</v>
       </c>
     </row>
     <row r="100">
@@ -1528,10 +1528,10 @@
         <v>98</v>
       </c>
       <c r="B100" t="n">
-        <v>-1.013118917235847</v>
+        <v>0.6957844459985409</v>
       </c>
       <c r="C100" t="n">
-        <v>0.7744723783640283</v>
+        <v>-1.334993941807255</v>
       </c>
     </row>
     <row r="101">
@@ -1539,10 +1539,10 @@
         <v>99</v>
       </c>
       <c r="B101" t="n">
-        <v>0.7863567224802747</v>
+        <v>-0.2988073625544497</v>
       </c>
       <c r="C101" t="n">
-        <v>-1.027276084442938</v>
+        <v>-0.4763227695763352</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the pandas book examples
</commit_message>
<xml_diff>
--- a/Pandas/pandas/ex2.xlsx
+++ b/Pandas/pandas/ex2.xlsx
@@ -450,10 +450,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>-0.6436936677321438</v>
+        <v>1.192379144208543</v>
       </c>
       <c r="C2" t="n">
-        <v>0.6048615524379573</v>
+        <v>1.020878496217309</v>
       </c>
     </row>
     <row r="3">
@@ -461,10 +461,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0.8481987922759403</v>
+        <v>1.869410725055877</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.06183975955357971</v>
+        <v>-1.281648130147154</v>
       </c>
     </row>
     <row r="4">
@@ -472,10 +472,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>0.1362243115762983</v>
+        <v>-0.3318649995207109</v>
       </c>
       <c r="C4" t="n">
-        <v>0.6668242860948045</v>
+        <v>0.5050772145142584</v>
       </c>
     </row>
     <row r="5">
@@ -483,10 +483,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>-2.866014234017723</v>
+        <v>0.5404290999940266</v>
       </c>
       <c r="C5" t="n">
-        <v>1.427542058963176</v>
+        <v>0.3944810077655069</v>
       </c>
     </row>
     <row r="6">
@@ -494,10 +494,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.4341914718821441</v>
+        <v>-2.075031836665305</v>
       </c>
       <c r="C6" t="n">
-        <v>-1.875270068897947</v>
+        <v>0.6967747618062374</v>
       </c>
     </row>
     <row r="7">
@@ -505,10 +505,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>-1.448678003288501</v>
+        <v>-0.5111026748439523</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.7410904468199772</v>
+        <v>1.258140074602792</v>
       </c>
     </row>
     <row r="8">
@@ -516,10 +516,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>-2.670841336409842</v>
+        <v>0.3199689044927579</v>
       </c>
       <c r="C8" t="n">
-        <v>0.3023040868638705</v>
+        <v>0.6547783786586647</v>
       </c>
     </row>
     <row r="9">
@@ -527,10 +527,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>0.253343792392148</v>
+        <v>-1.35617258160237</v>
       </c>
       <c r="C9" t="n">
-        <v>0.3395936605247907</v>
+        <v>0.2897668936346211</v>
       </c>
     </row>
     <row r="10">
@@ -538,10 +538,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>1.124378825728025</v>
+        <v>-1.759167151189836</v>
       </c>
       <c r="C10" t="n">
-        <v>0.5815546117344512</v>
+        <v>0.218972355154201</v>
       </c>
     </row>
     <row r="11">
@@ -549,10 +549,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>-0.3328171023833046</v>
+        <v>0.2081726550663906</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.734141001411168</v>
+        <v>-0.09762189235145383</v>
       </c>
     </row>
     <row r="12">
@@ -560,10 +560,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>0.9715251082647074</v>
+        <v>0.5739423672284978</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.5451462484222711</v>
+        <v>0.1173796061076274</v>
       </c>
     </row>
     <row r="13">
@@ -571,10 +571,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>-0.3151471034450695</v>
+        <v>0.5783484400170088</v>
       </c>
       <c r="C13" t="n">
-        <v>0.9682226724522393</v>
+        <v>2.253570470933922</v>
       </c>
     </row>
     <row r="14">
@@ -582,10 +582,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>-0.4595775492837924</v>
+        <v>-1.056023949464658</v>
       </c>
       <c r="C14" t="n">
-        <v>0.8289935256924429</v>
+        <v>1.521058393174677</v>
       </c>
     </row>
     <row r="15">
@@ -593,10 +593,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>0.6593929085579789</v>
+        <v>1.535231403256816</v>
       </c>
       <c r="C15" t="n">
-        <v>-2.243730152265649</v>
+        <v>-0.1210661790642925</v>
       </c>
     </row>
     <row r="16">
@@ -604,10 +604,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>-0.07791176058193165</v>
+        <v>1.386474917277614</v>
       </c>
       <c r="C16" t="n">
-        <v>-0.6495241628031473</v>
+        <v>0.4228447078699191</v>
       </c>
     </row>
     <row r="17">
@@ -615,10 +615,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>0.1686142624598296</v>
+        <v>1.622349763539734</v>
       </c>
       <c r="C17" t="n">
-        <v>0.191724201537998</v>
+        <v>-1.655081222885729</v>
       </c>
     </row>
     <row r="18">
@@ -626,10 +626,10 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>2.382645102519338</v>
+        <v>0.07375551398390523</v>
       </c>
       <c r="C18" t="n">
-        <v>-0.4582057661330416</v>
+        <v>2.744087149141673</v>
       </c>
     </row>
     <row r="19">
@@ -637,10 +637,10 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>0.550240542470282</v>
+        <v>0.5887235888409346</v>
       </c>
       <c r="C19" t="n">
-        <v>1.436781058176872</v>
+        <v>-1.503518955136582</v>
       </c>
     </row>
     <row r="20">
@@ -648,10 +648,10 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>-1.32313431129281</v>
+        <v>0.2329519635282597</v>
       </c>
       <c r="C20" t="n">
-        <v>-2.230893663151085</v>
+        <v>1.312606378596723</v>
       </c>
     </row>
     <row r="21">
@@ -659,10 +659,10 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>0.1201625389229685</v>
+        <v>0.6977626795966044</v>
       </c>
       <c r="C21" t="n">
-        <v>0.6169262894177493</v>
+        <v>-0.4454913566412553</v>
       </c>
     </row>
     <row r="22">
@@ -670,10 +670,10 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>-1.238371232078775</v>
+        <v>-7.823961179193332e-05</v>
       </c>
       <c r="C22" t="n">
-        <v>-0.3955137710785661</v>
+        <v>0.8118579174230005</v>
       </c>
     </row>
     <row r="23">
@@ -681,10 +681,10 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>-1.794652629800652</v>
+        <v>-0.3209752567494464</v>
       </c>
       <c r="C23" t="n">
-        <v>2.468249722939703</v>
+        <v>1.32721658784677</v>
       </c>
     </row>
     <row r="24">
@@ -692,10 +692,10 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>-0.0836666869437588</v>
+        <v>-2.731244840337007</v>
       </c>
       <c r="C24" t="n">
-        <v>-0.9638709116197721</v>
+        <v>0.2206305342992531</v>
       </c>
     </row>
     <row r="25">
@@ -703,10 +703,10 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>-1.479878989264926</v>
+        <v>-0.6388527528244204</v>
       </c>
       <c r="C25" t="n">
-        <v>0.3508202005104995</v>
+        <v>0.6918707534773548</v>
       </c>
     </row>
     <row r="26">
@@ -714,10 +714,10 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>1.482014008149077</v>
+        <v>-0.2368370806480016</v>
       </c>
       <c r="C26" t="n">
-        <v>0.7554382049861887</v>
+        <v>-1.098004355100295</v>
       </c>
     </row>
     <row r="27">
@@ -725,10 +725,10 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>-0.4152403562579223</v>
+        <v>1.340773809355093</v>
       </c>
       <c r="C27" t="n">
-        <v>1.148642674641205</v>
+        <v>-0.5214057232960154</v>
       </c>
     </row>
     <row r="28">
@@ -736,10 +736,10 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>1.123590593476252</v>
+        <v>0.1359954553019375</v>
       </c>
       <c r="C28" t="n">
-        <v>-1.060910880374953</v>
+        <v>-1.475737748515807</v>
       </c>
     </row>
     <row r="29">
@@ -747,10 +747,10 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>0.1594692143239325</v>
+        <v>-0.991772331957005</v>
       </c>
       <c r="C29" t="n">
-        <v>1.221488544430398</v>
+        <v>-0.3836665694253608</v>
       </c>
     </row>
     <row r="30">
@@ -758,10 +758,10 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>-0.2933732025751061</v>
+        <v>1.611006750604784</v>
       </c>
       <c r="C30" t="n">
-        <v>-0.214152447243255</v>
+        <v>0.2387426199344161</v>
       </c>
     </row>
     <row r="31">
@@ -769,10 +769,10 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>-0.8855557045211763</v>
+        <v>1.13992759312113</v>
       </c>
       <c r="C31" t="n">
-        <v>1.020915229079611</v>
+        <v>-1.050319633043887</v>
       </c>
     </row>
     <row r="32">
@@ -780,10 +780,10 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>0.0620496432929693</v>
+        <v>-1.833060252516225</v>
       </c>
       <c r="C32" t="n">
-        <v>0.3544165865739892</v>
+        <v>-1.08054182651166</v>
       </c>
     </row>
     <row r="33">
@@ -791,10 +791,10 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>-1.3702988547915</v>
+        <v>0.3698471364797039</v>
       </c>
       <c r="C33" t="n">
-        <v>-0.6461119001904715</v>
+        <v>-0.5544481275710363</v>
       </c>
     </row>
     <row r="34">
@@ -802,10 +802,10 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>-1.754582786087739</v>
+        <v>0.4843941365775502</v>
       </c>
       <c r="C34" t="n">
-        <v>-0.3991244150749291</v>
+        <v>0.4540101986283487</v>
       </c>
     </row>
     <row r="35">
@@ -813,10 +813,10 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>0.5664072676744579</v>
+        <v>1.312609627433891</v>
       </c>
       <c r="C35" t="n">
-        <v>-1.480385013511401</v>
+        <v>-0.9707706091423735</v>
       </c>
     </row>
     <row r="36">
@@ -824,10 +824,10 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>1.445166997699438</v>
+        <v>0.2643944700618042</v>
       </c>
       <c r="C36" t="n">
-        <v>-1.639949060347753</v>
+        <v>1.052694640878439</v>
       </c>
     </row>
     <row r="37">
@@ -835,10 +835,10 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>0.4459971448962949</v>
+        <v>0.917289058043892</v>
       </c>
       <c r="C37" t="n">
-        <v>-0.5379657233611839</v>
+        <v>-0.02152797604127773</v>
       </c>
     </row>
     <row r="38">
@@ -846,10 +846,10 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>-1.565073502983542</v>
+        <v>-1.217913137748882</v>
       </c>
       <c r="C38" t="n">
-        <v>-0.6950834099672214</v>
+        <v>-1.74789066163599</v>
       </c>
     </row>
     <row r="39">
@@ -857,10 +857,10 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>0.2463880731422886</v>
+        <v>-1.248966940002415</v>
       </c>
       <c r="C39" t="n">
-        <v>-0.2477069577402639</v>
+        <v>-0.9343346199714787</v>
       </c>
     </row>
     <row r="40">
@@ -868,10 +868,10 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>-0.3507242913887475</v>
+        <v>0.3997025630753042</v>
       </c>
       <c r="C40" t="n">
-        <v>-1.44051868664003</v>
+        <v>-0.5442632709721983</v>
       </c>
     </row>
     <row r="41">
@@ -879,10 +879,10 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>-0.6514460131826214</v>
+        <v>-0.8439833737238367</v>
       </c>
       <c r="C41" t="n">
-        <v>-0.6292782376388897</v>
+        <v>-0.6695234394738477</v>
       </c>
     </row>
     <row r="42">
@@ -890,10 +890,10 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>-0.5464757699054879</v>
+        <v>1.420299377282191</v>
       </c>
       <c r="C42" t="n">
-        <v>-0.1714765588734759</v>
+        <v>-0.05948106311461374</v>
       </c>
     </row>
     <row r="43">
@@ -901,10 +901,10 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>0.3231629392285399</v>
+        <v>-1.047372510070521</v>
       </c>
       <c r="C43" t="n">
-        <v>0.6534159802800087</v>
+        <v>0.4643097799862644</v>
       </c>
     </row>
     <row r="44">
@@ -912,10 +912,10 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>-0.2915282051470537</v>
+        <v>0.4492618213325623</v>
       </c>
       <c r="C44" t="n">
-        <v>0.6967750831528265</v>
+        <v>1.164543727404403</v>
       </c>
     </row>
     <row r="45">
@@ -923,10 +923,10 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>0.6151820722118405</v>
+        <v>-1.438805797647627</v>
       </c>
       <c r="C45" t="n">
-        <v>1.091175472278164</v>
+        <v>1.118274495760478</v>
       </c>
     </row>
     <row r="46">
@@ -934,10 +934,10 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>2.588000478193001</v>
+        <v>0.04325537894974833</v>
       </c>
       <c r="C46" t="n">
-        <v>-0.04589524596991784</v>
+        <v>0.7692194348056423</v>
       </c>
     </row>
     <row r="47">
@@ -945,10 +945,10 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>1.370749451107059</v>
+        <v>0.8948883800423968</v>
       </c>
       <c r="C47" t="n">
-        <v>-1.178660215603311</v>
+        <v>0.9529118303795087</v>
       </c>
     </row>
     <row r="48">
@@ -956,10 +956,10 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>0.9393252668458343</v>
+        <v>0.7121364849840244</v>
       </c>
       <c r="C48" t="n">
-        <v>-1.355580438879415</v>
+        <v>-0.3280813682164516</v>
       </c>
     </row>
     <row r="49">
@@ -967,10 +967,10 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>0.3006316064031579</v>
+        <v>-0.3144437777077964</v>
       </c>
       <c r="C49" t="n">
-        <v>0.771349844936364</v>
+        <v>-1.037981949723861</v>
       </c>
     </row>
     <row r="50">
@@ -978,10 +978,10 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>0.05815274417296564</v>
+        <v>0.2958377521785464</v>
       </c>
       <c r="C50" t="n">
-        <v>2.246041315098033</v>
+        <v>0.6952632191266608</v>
       </c>
     </row>
     <row r="51">
@@ -989,10 +989,10 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>0.5267149621358643</v>
+        <v>-0.4683944943133739</v>
       </c>
       <c r="C51" t="n">
-        <v>0.8233417008525109</v>
+        <v>1.973283416132937</v>
       </c>
     </row>
     <row r="52">
@@ -1000,10 +1000,10 @@
         <v>50</v>
       </c>
       <c r="B52" t="n">
-        <v>-0.7123731816434228</v>
+        <v>0.9765061533991062</v>
       </c>
       <c r="C52" t="n">
-        <v>0.276469818975218</v>
+        <v>-0.09018112569116743</v>
       </c>
     </row>
     <row r="53">
@@ -1011,10 +1011,10 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>0.8581973449076185</v>
+        <v>-0.8189111800306275</v>
       </c>
       <c r="C53" t="n">
-        <v>0.2413355351084589</v>
+        <v>-0.5348616149443042</v>
       </c>
     </row>
     <row r="54">
@@ -1022,10 +1022,10 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>-1.145956704531524</v>
+        <v>0.7984055820872634</v>
       </c>
       <c r="C54" t="n">
-        <v>-1.226158624623136</v>
+        <v>0.7821310160777513</v>
       </c>
     </row>
     <row r="55">
@@ -1033,10 +1033,10 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>0.5361686707597</v>
+        <v>-0.983976102206072</v>
       </c>
       <c r="C55" t="n">
-        <v>-0.2499597238895034</v>
+        <v>-0.144608738519537</v>
       </c>
     </row>
     <row r="56">
@@ -1044,10 +1044,10 @@
         <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>0.7660601344380447</v>
+        <v>1.270571652332778</v>
       </c>
       <c r="C56" t="n">
-        <v>0.6634042422292832</v>
+        <v>1.765715213971919</v>
       </c>
     </row>
     <row r="57">
@@ -1055,10 +1055,10 @@
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>-0.9432762958309731</v>
+        <v>-0.006603034504613346</v>
       </c>
       <c r="C57" t="n">
-        <v>0.2823738417461684</v>
+        <v>-0.286719414443142</v>
       </c>
     </row>
     <row r="58">
@@ -1066,10 +1066,10 @@
         <v>56</v>
       </c>
       <c r="B58" t="n">
-        <v>-0.837221143630809</v>
+        <v>-0.4017324373319931</v>
       </c>
       <c r="C58" t="n">
-        <v>-0.8561477056658795</v>
+        <v>0.5249819995714261</v>
       </c>
     </row>
     <row r="59">
@@ -1077,10 +1077,10 @@
         <v>57</v>
       </c>
       <c r="B59" t="n">
-        <v>-0.8351698402828253</v>
+        <v>0.04851654211596454</v>
       </c>
       <c r="C59" t="n">
-        <v>0.8263068678054736</v>
+        <v>-1.512763887543003</v>
       </c>
     </row>
     <row r="60">
@@ -1088,10 +1088,10 @@
         <v>58</v>
       </c>
       <c r="B60" t="n">
-        <v>0.1419408932370512</v>
+        <v>-1.339533302091071</v>
       </c>
       <c r="C60" t="n">
-        <v>-1.495064388596024</v>
+        <v>0.6738325834995891</v>
       </c>
     </row>
     <row r="61">
@@ -1099,10 +1099,10 @@
         <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>0.3022392408561329</v>
+        <v>0.9246830352672981</v>
       </c>
       <c r="C61" t="n">
-        <v>-0.3825669144857662</v>
+        <v>-0.1077531474302199</v>
       </c>
     </row>
     <row r="62">
@@ -1110,10 +1110,10 @@
         <v>60</v>
       </c>
       <c r="B62" t="n">
-        <v>-0.4127490461341597</v>
+        <v>-0.362427718590265</v>
       </c>
       <c r="C62" t="n">
-        <v>-0.6458329774761561</v>
+        <v>0.2632869405297432</v>
       </c>
     </row>
     <row r="63">
@@ -1121,10 +1121,10 @@
         <v>61</v>
       </c>
       <c r="B63" t="n">
-        <v>-2.085492571584192</v>
+        <v>0.1186266454692196</v>
       </c>
       <c r="C63" t="n">
-        <v>0.3716365098571095</v>
+        <v>-0.4215271135205001</v>
       </c>
     </row>
     <row r="64">
@@ -1132,10 +1132,10 @@
         <v>62</v>
       </c>
       <c r="B64" t="n">
-        <v>0.1315193023423922</v>
+        <v>-1.188002100962399</v>
       </c>
       <c r="C64" t="n">
-        <v>1.222406872154715</v>
+        <v>0.6673674908628129</v>
       </c>
     </row>
     <row r="65">
@@ -1143,10 +1143,10 @@
         <v>63</v>
       </c>
       <c r="B65" t="n">
-        <v>-0.2386606521516989</v>
+        <v>-1.880628233888685</v>
       </c>
       <c r="C65" t="n">
-        <v>0.5866952124266063</v>
+        <v>-0.1978679876255</v>
       </c>
     </row>
     <row r="66">
@@ -1154,10 +1154,10 @@
         <v>64</v>
       </c>
       <c r="B66" t="n">
-        <v>0.2617963838242409</v>
+        <v>-1.77824547667701</v>
       </c>
       <c r="C66" t="n">
-        <v>0.06977936609247397</v>
+        <v>-0.9849916834864952</v>
       </c>
     </row>
     <row r="67">
@@ -1165,10 +1165,10 @@
         <v>65</v>
       </c>
       <c r="B67" t="n">
-        <v>-0.6241851056429294</v>
+        <v>-0.2613510960543449</v>
       </c>
       <c r="C67" t="n">
-        <v>-1.037653362277436</v>
+        <v>-1.418749517929991</v>
       </c>
     </row>
     <row r="68">
@@ -1176,10 +1176,10 @@
         <v>66</v>
       </c>
       <c r="B68" t="n">
-        <v>-0.4539420747994777</v>
+        <v>-0.8594230303627027</v>
       </c>
       <c r="C68" t="n">
-        <v>1.30576054228318</v>
+        <v>-0.9594827179566222</v>
       </c>
     </row>
     <row r="69">
@@ -1187,10 +1187,10 @@
         <v>67</v>
       </c>
       <c r="B69" t="n">
-        <v>-0.404701238277281</v>
+        <v>-1.502826027541549</v>
       </c>
       <c r="C69" t="n">
-        <v>1.075223412767373</v>
+        <v>-0.9131374486911226</v>
       </c>
     </row>
     <row r="70">
@@ -1198,10 +1198,10 @@
         <v>68</v>
       </c>
       <c r="B70" t="n">
-        <v>1.235252177085605</v>
+        <v>-0.8280475372669485</v>
       </c>
       <c r="C70" t="n">
-        <v>-0.8031512192257261</v>
+        <v>-0.09310227790034203</v>
       </c>
     </row>
     <row r="71">
@@ -1209,10 +1209,10 @@
         <v>69</v>
       </c>
       <c r="B71" t="n">
-        <v>0.09702201463857606</v>
+        <v>-0.4875854510153331</v>
       </c>
       <c r="C71" t="n">
-        <v>1.453845934993659</v>
+        <v>-0.7386467929429651</v>
       </c>
     </row>
     <row r="72">
@@ -1220,10 +1220,10 @@
         <v>70</v>
       </c>
       <c r="B72" t="n">
-        <v>-0.09487154581914876</v>
+        <v>2.249225385225403</v>
       </c>
       <c r="C72" t="n">
-        <v>1.814408098157268</v>
+        <v>0.6157045521350214</v>
       </c>
     </row>
     <row r="73">
@@ -1231,10 +1231,10 @@
         <v>71</v>
       </c>
       <c r="B73" t="n">
-        <v>0.2271801367917244</v>
+        <v>-0.536050976682898</v>
       </c>
       <c r="C73" t="n">
-        <v>-1.115393088223188</v>
+        <v>0.8398493684103168</v>
       </c>
     </row>
     <row r="74">
@@ -1242,10 +1242,10 @@
         <v>72</v>
       </c>
       <c r="B74" t="n">
-        <v>0.9328267110342523</v>
+        <v>-0.000259126682991129</v>
       </c>
       <c r="C74" t="n">
-        <v>2.168521318056309</v>
+        <v>-0.4070462846514331</v>
       </c>
     </row>
     <row r="75">
@@ -1253,10 +1253,10 @@
         <v>73</v>
       </c>
       <c r="B75" t="n">
-        <v>-0.09315705105604782</v>
+        <v>-1.345807542313552</v>
       </c>
       <c r="C75" t="n">
-        <v>-0.345436021703852</v>
+        <v>-0.3326405680186354</v>
       </c>
     </row>
     <row r="76">
@@ -1264,10 +1264,10 @@
         <v>74</v>
       </c>
       <c r="B76" t="n">
-        <v>1.878318642470408</v>
+        <v>-0.8882895590503391</v>
       </c>
       <c r="C76" t="n">
-        <v>1.116318477641528</v>
+        <v>0.6005608808997036</v>
       </c>
     </row>
     <row r="77">
@@ -1275,10 +1275,10 @@
         <v>75</v>
       </c>
       <c r="B77" t="n">
-        <v>0.1932647763661189</v>
+        <v>0.06485664618251867</v>
       </c>
       <c r="C77" t="n">
-        <v>-0.5724231192636764</v>
+        <v>-1.848934592689371</v>
       </c>
     </row>
     <row r="78">
@@ -1286,10 +1286,10 @@
         <v>76</v>
       </c>
       <c r="B78" t="n">
-        <v>0.1912617951639147</v>
+        <v>-0.8578388197711537</v>
       </c>
       <c r="C78" t="n">
-        <v>-0.6834481631749896</v>
+        <v>-0.3237962582991278</v>
       </c>
     </row>
     <row r="79">
@@ -1297,10 +1297,10 @@
         <v>77</v>
       </c>
       <c r="B79" t="n">
-        <v>-0.2693225846762528</v>
+        <v>0.5109079369671307</v>
       </c>
       <c r="C79" t="n">
-        <v>0.4378468894079781</v>
+        <v>1.320044902279415</v>
       </c>
     </row>
     <row r="80">
@@ -1308,10 +1308,10 @@
         <v>78</v>
       </c>
       <c r="B80" t="n">
-        <v>0.5623434878191472</v>
+        <v>-0.07868143035309444</v>
       </c>
       <c r="C80" t="n">
-        <v>0.3404363215159713</v>
+        <v>-0.9024747160414333</v>
       </c>
     </row>
     <row r="81">
@@ -1319,10 +1319,10 @@
         <v>79</v>
       </c>
       <c r="B81" t="n">
-        <v>-0.8391119319658223</v>
+        <v>0.7042676453403998</v>
       </c>
       <c r="C81" t="n">
-        <v>-1.456319730170735</v>
+        <v>0.37959750313202</v>
       </c>
     </row>
     <row r="82">
@@ -1330,10 +1330,10 @@
         <v>80</v>
       </c>
       <c r="B82" t="n">
-        <v>-1.948869760072637</v>
+        <v>0.1676812134989119</v>
       </c>
       <c r="C82" t="n">
-        <v>-0.1042592799032529</v>
+        <v>-0.3774515159114227</v>
       </c>
     </row>
     <row r="83">
@@ -1341,10 +1341,10 @@
         <v>81</v>
       </c>
       <c r="B83" t="n">
-        <v>-1.44804662971959</v>
+        <v>0.08772380717624008</v>
       </c>
       <c r="C83" t="n">
-        <v>-0.02036165746055315</v>
+        <v>-0.3230851048635872</v>
       </c>
     </row>
     <row r="84">
@@ -1352,10 +1352,10 @@
         <v>82</v>
       </c>
       <c r="B84" t="n">
-        <v>0.06947472423285476</v>
+        <v>-0.4055975553642957</v>
       </c>
       <c r="C84" t="n">
-        <v>0.3447790295087322</v>
+        <v>1.183736920463053</v>
       </c>
     </row>
     <row r="85">
@@ -1363,10 +1363,10 @@
         <v>83</v>
       </c>
       <c r="B85" t="n">
-        <v>0.03229711418411784</v>
+        <v>-0.2536159307640937</v>
       </c>
       <c r="C85" t="n">
-        <v>-1.180213158933638</v>
+        <v>0.1954726169814617</v>
       </c>
     </row>
     <row r="86">
@@ -1374,10 +1374,10 @@
         <v>84</v>
       </c>
       <c r="B86" t="n">
-        <v>-0.03350886978972536</v>
+        <v>-0.6021080182295203</v>
       </c>
       <c r="C86" t="n">
-        <v>0.03624222666411998</v>
+        <v>0.3503202793467673</v>
       </c>
     </row>
     <row r="87">
@@ -1385,10 +1385,10 @@
         <v>85</v>
       </c>
       <c r="B87" t="n">
-        <v>0.7344473818902533</v>
+        <v>-0.8334508237560108</v>
       </c>
       <c r="C87" t="n">
-        <v>-0.510248074893689</v>
+        <v>-1.152132544257979</v>
       </c>
     </row>
     <row r="88">
@@ -1396,10 +1396,10 @@
         <v>86</v>
       </c>
       <c r="B88" t="n">
-        <v>-1.092627473367835</v>
+        <v>-1.304848672330186</v>
       </c>
       <c r="C88" t="n">
-        <v>-0.7863097810137865</v>
+        <v>0.07460410023412248</v>
       </c>
     </row>
     <row r="89">
@@ -1407,10 +1407,10 @@
         <v>87</v>
       </c>
       <c r="B89" t="n">
-        <v>0.5658131615087325</v>
+        <v>-1.537519732787598</v>
       </c>
       <c r="C89" t="n">
-        <v>1.195582748791698</v>
+        <v>-0.07064307351042641</v>
       </c>
     </row>
     <row r="90">
@@ -1418,10 +1418,10 @@
         <v>88</v>
       </c>
       <c r="B90" t="n">
-        <v>0.755411988513544</v>
+        <v>-0.5991997288862755</v>
       </c>
       <c r="C90" t="n">
-        <v>0.1232495374633156</v>
+        <v>0.1930999299518052</v>
       </c>
     </row>
     <row r="91">
@@ -1429,10 +1429,10 @@
         <v>89</v>
       </c>
       <c r="B91" t="n">
-        <v>-0.678145361754754</v>
+        <v>1.881840816077361</v>
       </c>
       <c r="C91" t="n">
-        <v>-1.102240414597044</v>
+        <v>-0.1616931509889499</v>
       </c>
     </row>
     <row r="92">
@@ -1440,10 +1440,10 @@
         <v>90</v>
       </c>
       <c r="B92" t="n">
-        <v>-1.916282923517614</v>
+        <v>0.850594307374502</v>
       </c>
       <c r="C92" t="n">
-        <v>0.7102227163283419</v>
+        <v>-0.130687638173106</v>
       </c>
     </row>
     <row r="93">
@@ -1451,10 +1451,10 @@
         <v>91</v>
       </c>
       <c r="B93" t="n">
-        <v>-0.8248177828102289</v>
+        <v>0.06328323988962521</v>
       </c>
       <c r="C93" t="n">
-        <v>0.3554956757573015</v>
+        <v>-0.2647791550849387</v>
       </c>
     </row>
     <row r="94">
@@ -1462,10 +1462,10 @@
         <v>92</v>
       </c>
       <c r="B94" t="n">
-        <v>1.228226554465794</v>
+        <v>-0.1134089336824713</v>
       </c>
       <c r="C94" t="n">
-        <v>0.03827843410827805</v>
+        <v>0.02299509973896885</v>
       </c>
     </row>
     <row r="95">
@@ -1473,10 +1473,10 @@
         <v>93</v>
       </c>
       <c r="B95" t="n">
-        <v>-0.5431044208630181</v>
+        <v>0.9799009882876903</v>
       </c>
       <c r="C95" t="n">
-        <v>-1.12796578461849</v>
+        <v>0.4164063954553908</v>
       </c>
     </row>
     <row r="96">
@@ -1484,10 +1484,10 @@
         <v>94</v>
       </c>
       <c r="B96" t="n">
-        <v>0.3684630369346275</v>
+        <v>-1.715323537310211</v>
       </c>
       <c r="C96" t="n">
-        <v>1.277668742749809</v>
+        <v>1.405001459122823</v>
       </c>
     </row>
     <row r="97">
@@ -1495,10 +1495,10 @@
         <v>95</v>
       </c>
       <c r="B97" t="n">
-        <v>1.287616710102915</v>
+        <v>0.1566327268391177</v>
       </c>
       <c r="C97" t="n">
-        <v>-0.5011707599454829</v>
+        <v>0.2459133845969255</v>
       </c>
     </row>
     <row r="98">
@@ -1506,10 +1506,10 @@
         <v>96</v>
       </c>
       <c r="B98" t="n">
-        <v>-0.07176661507610869</v>
+        <v>-0.432329694715788</v>
       </c>
       <c r="C98" t="n">
-        <v>1.301262065439911</v>
+        <v>-0.3299313555613803</v>
       </c>
     </row>
     <row r="99">
@@ -1517,10 +1517,10 @@
         <v>97</v>
       </c>
       <c r="B99" t="n">
-        <v>0.7745833125790254</v>
+        <v>1.285364363937007</v>
       </c>
       <c r="C99" t="n">
-        <v>-0.7349295588644752</v>
+        <v>0.9261455694758151</v>
       </c>
     </row>
     <row r="100">
@@ -1528,10 +1528,10 @@
         <v>98</v>
       </c>
       <c r="B100" t="n">
-        <v>0.6957844459985409</v>
+        <v>-0.5035318536672438</v>
       </c>
       <c r="C100" t="n">
-        <v>-1.334993941807255</v>
+        <v>0.3242433330753783</v>
       </c>
     </row>
     <row r="101">
@@ -1539,10 +1539,10 @@
         <v>99</v>
       </c>
       <c r="B101" t="n">
-        <v>-0.2988073625544497</v>
+        <v>-0.6592318622190665</v>
       </c>
       <c r="C101" t="n">
-        <v>-0.4763227695763352</v>
+        <v>-0.6887154276976315</v>
       </c>
     </row>
   </sheetData>

</xml_diff>